<commit_message>
Added till 23/04/2021[Week 4 completed]
</commit_message>
<xml_diff>
--- a/Week 4/Week 4 Plan.xlsx
+++ b/Week 4/Week 4 Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA\Week 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F727AC-6E7C-4729-9DC4-6895018048F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD055A4-137F-487E-9A3E-B0A1E89050BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Linked list Questions</t>
   </si>
@@ -170,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -192,6 +192,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,13 +419,14 @@
   <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="101" style="3" customWidth="1"/>
-    <col min="2" max="16384" width="14.44140625" style="3"/>
+    <col min="2" max="2" width="14.44140625" style="12"/>
+    <col min="3" max="16384" width="14.44140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -470,7 +477,9 @@
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="C3" s="6"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -490,7 +499,9 @@
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="C4" s="6"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -510,7 +521,9 @@
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="C5" s="6"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -530,7 +543,9 @@
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="C6" s="6"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -550,7 +565,9 @@
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="C7" s="6"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -592,7 +609,9 @@
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -612,7 +631,7 @@
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -632,7 +651,9 @@
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -652,7 +673,9 @@
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -672,7 +695,7 @@
       <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="6"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -692,7 +715,9 @@
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -712,7 +737,7 @@
       <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -732,7 +757,7 @@
       <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="8"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -750,7 +775,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="8"/>
+      <c r="B17" s="9"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
@@ -768,7 +793,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="8"/>
+      <c r="B18" s="9"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -786,7 +811,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
-      <c r="B19" s="8"/>
+      <c r="B19" s="9"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -804,7 +829,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="8"/>
+      <c r="B20" s="9"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
@@ -822,7 +847,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
-      <c r="B21" s="8"/>
+      <c r="B21" s="9"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -840,7 +865,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
-      <c r="B22" s="8"/>
+      <c r="B22" s="9"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -858,7 +883,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
-      <c r="B23" s="8"/>
+      <c r="B23" s="9"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
@@ -876,7 +901,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="8"/>
+      <c r="B24" s="9"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
@@ -894,7 +919,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-      <c r="B25" s="8"/>
+      <c r="B25" s="9"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
@@ -912,7 +937,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="B26" s="8"/>
+      <c r="B26" s="9"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
@@ -930,7 +955,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
-      <c r="B27" s="8"/>
+      <c r="B27" s="9"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
@@ -948,7 +973,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="B28" s="8"/>
+      <c r="B28" s="9"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>

</xml_diff>